<commit_message>
draft of NL regression with slope calculations
</commit_message>
<xml_diff>
--- a/biochemist-python/chapters/data/enzyme_kinetics.xlsx
+++ b/biochemist-python/chapters/data/enzyme_kinetics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pac8612/Desktop/python-scripting-biochemistry/biochemist-python/chapters/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4CD02D-B706-2B44-9F4E-76A88F24DD79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7A210B-72EA-2945-B987-C5F2DAFB7934}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37560" yWindow="3980" windowWidth="30200" windowHeight="17020" xr2:uid="{7FC78297-7CA3-BA42-ABA4-A8E2D6909EAB}"/>
+    <workbookView xWindow="1680" yWindow="3320" windowWidth="30200" windowHeight="17020" xr2:uid="{7FC78297-7CA3-BA42-ABA4-A8E2D6909EAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2327,64 +2327,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>7.3923444976076558E-2</c:v>
+                  <c:v>7.320574162679426E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14928229665071771</c:v>
+                  <c:v>0.14784688995215312</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22392344497607655</c:v>
+                  <c:v>0.22177033492822965</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2755980861244019</c:v>
+                  <c:v>0.29282296650717704</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35885167464114831</c:v>
+                  <c:v>0.36602870813397126</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.44354066985645929</c:v>
+                  <c:v>0.40909090909090906</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51244019138755981</c:v>
+                  <c:v>0.52751196172248804</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.56267942583732056</c:v>
+                  <c:v>0.58564593301435408</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.63947368421052631</c:v>
+                  <c:v>0.61363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.68181818181818177</c:v>
+                  <c:v>0.75358851674641147</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.82894736842105265</c:v>
+                  <c:v>0.78157894736842104</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.87846889952153107</c:v>
+                  <c:v>0.84401913875598078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.91435406698564592</c:v>
+                  <c:v>0.88636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0349282296650717</c:v>
+                  <c:v>1.0449760765550238</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1.0334928229665072</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1712918660287082</c:v>
+                  <c:v>1.1253588516746411</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1712918660287079</c:v>
+                  <c:v>1.1956937799043061</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.2789473684210526</c:v>
+                  <c:v>1.3306220095693782</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.4318181818181817</c:v>
+                  <c:v>1.418181818181818</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.4784688995215309</c:v>
+                  <c:v>1.5071770334928229</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2487,64 +2487,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>6.8807339449541288E-2</c:v>
+                  <c:v>7.087155963302752E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13486238532110092</c:v>
+                  <c:v>0.13211009174311927</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21467889908256879</c:v>
+                  <c:v>0.19610091743119265</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26697247706422023</c:v>
+                  <c:v>0.26422018348623855</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34059633027522934</c:v>
+                  <c:v>0.34747706422018348</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4211009174311926</c:v>
+                  <c:v>0.41284403669724767</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49128440366972481</c:v>
+                  <c:v>0.48165137614678905</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.54495412844036695</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61926605504587151</c:v>
+                  <c:v>0.6316513761467889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.65366972477064222</c:v>
+                  <c:v>0.72247706422018343</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.726605504587156</c:v>
+                  <c:v>0.74931192660550461</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.82568807339449535</c:v>
+                  <c:v>0.83394495412844027</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.87660550458715591</c:v>
+                  <c:v>0.88555045871559634</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.95366972477064227</c:v>
+                  <c:v>0.92477064220183491</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0114678899082568</c:v>
+                  <c:v>1.0837155963302751</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0568807339449542</c:v>
+                  <c:v>1.0788990825688074</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1580275229357797</c:v>
+                  <c:v>1.2048165137614679</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.1889908256880732</c:v>
+                  <c:v>1.2633027522935778</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.3727064220183487</c:v>
+                  <c:v>1.3596330275229358</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.3623853211009174</c:v>
+                  <c:v>1.3211009174311927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2659,64 +2659,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>6.5791139240506322E-2</c:v>
+                  <c:v>6.7784810126582273E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13424050632911391</c:v>
+                  <c:v>0.13158227848101264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20534810126582276</c:v>
+                  <c:v>0.20734177215189872</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.26316455696202529</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34556962025316451</c:v>
+                  <c:v>0.33892405063291131</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37879746835443034</c:v>
+                  <c:v>0.41468354430379745</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.48379746835443038</c:v>
+                  <c:v>0.45123417721518988</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.54227848101265819</c:v>
+                  <c:v>0.5156962025316455</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61604430379746833</c:v>
+                  <c:v>0.59212025316455696</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.69113924050632902</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.72370253164556952</c:v>
+                  <c:v>0.7602531645569619</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.78151898734177205</c:v>
+                  <c:v>0.78949367088607592</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.82072784810126576</c:v>
+                  <c:v>0.88120253164556961</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.95829113924050624</c:v>
+                  <c:v>0.92107594936708859</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.99683544303797456</c:v>
+                  <c:v>1.0367088607594936</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0739240506329113</c:v>
+                  <c:v>1.0101265822784808</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1862341772151896</c:v>
+                  <c:v>1.1749367088607592</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.2081645569620252</c:v>
+                  <c:v>1.136392405063291</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2374050632911391</c:v>
+                  <c:v>1.3131645569620252</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.3025316455696201</c:v>
+                  <c:v>1.2759493670886073</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2834,61 +2834,61 @@
                   <c:v>5.8163265306122446E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1273469387755102</c:v>
+                  <c:v>0.12612244897959182</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18183673469387757</c:v>
+                  <c:v>0.19285714285714287</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24</c:v>
+                  <c:v>0.2473469387755102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.29081632653061223</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.36734693877551022</c:v>
+                  <c:v>0.3563265306122449</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43285714285714288</c:v>
+                  <c:v>0.43714285714285717</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.48489795918367345</c:v>
+                  <c:v>0.4946938775510204</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.54</c:v>
+                  <c:v>0.5234693877551021</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61224489795918369</c:v>
+                  <c:v>0.61836734693877549</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.69367346938775509</c:v>
+                  <c:v>0.63979591836734695</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.69795918367346943</c:v>
+                  <c:v>0.7567346938775511</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.80387755102040814</c:v>
+                  <c:v>0.79591836734693877</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.81428571428571439</c:v>
+                  <c:v>0.84857142857142864</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.89081632653061216</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.9893877551020408</c:v>
+                  <c:v>0.94040816326530607</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0304081632653059</c:v>
+                  <c:v>1.0199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.08</c:v>
+                  <c:v>1.0469387755102042</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2214285714285713</c:v>
+                  <c:v>1.1516326530612244</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.2122448979591838</c:v>
+                  <c:v>1.1632653061224489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2991,64 +2991,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>4.9655172413793101E-2</c:v>
+                  <c:v>5.3275862068965514E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10758620689655173</c:v>
+                  <c:v>0.10655172413793103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15051724137931036</c:v>
+                  <c:v>0.15362068965517242</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19655172413793104</c:v>
+                  <c:v>0.20689655172413793</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25862068965517243</c:v>
+                  <c:v>0.26120689655172413</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30103448275862071</c:v>
+                  <c:v>0.29482758620689659</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.34396551724137936</c:v>
+                  <c:v>0.35120689655172421</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.41379310344827586</c:v>
+                  <c:v>0.43448275862068964</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47017241379310343</c:v>
+                  <c:v>0.44689655172413789</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.52758620689655178</c:v>
+                  <c:v>0.50689655172413794</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.58603448275862069</c:v>
+                  <c:v>0.59172413793103451</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.64551724137931032</c:v>
+                  <c:v>0.60827586206896556</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.66568965517241385</c:v>
+                  <c:v>0.6925862068965517</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.69517241379310357</c:v>
+                  <c:v>0.72413793103448287</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.75258620689655176</c:v>
+                  <c:v>0.7448275862068966</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.79448275862068962</c:v>
+                  <c:v>0.86896551724137927</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.90568965517241384</c:v>
+                  <c:v>0.83534482758620698</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.96827586206896554</c:v>
+                  <c:v>0.91241379310344828</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.98275862068965525</c:v>
+                  <c:v>1.0024137931034482</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0758620689655174</c:v>
+                  <c:v>1.0241379310344829</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3166,61 +3166,61 @@
                   <c:v>4.0263157894736848E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8947368421052641E-2</c:v>
+                  <c:v>7.5000000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12197368421052632</c:v>
+                  <c:v>0.12315789473684212</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16105263157894739</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20131578947368423</c:v>
+                  <c:v>0.19736842105263158</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23684210526315791</c:v>
+                  <c:v>0.24631578947368424</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27907894736842109</c:v>
+                  <c:v>0.28460526315789475</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.30947368421052635</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.35526315789473684</c:v>
+                  <c:v>0.34460526315789475</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.38289473684210529</c:v>
+                  <c:v>0.39473684210526316</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.44289473684210529</c:v>
+                  <c:v>0.43855263157894736</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.45947368421052637</c:v>
+                  <c:v>0.45473684210526316</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.52342105263157901</c:v>
+                  <c:v>0.50802631578947377</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.54157894736842116</c:v>
+                  <c:v>0.56368421052631579</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.62171052631578938</c:v>
+                  <c:v>0.5625</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.63789473684210529</c:v>
+                  <c:v>0.63157894736842113</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.65763157894736846</c:v>
+                  <c:v>0.69789473684210535</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.70342105263157895</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.74250000000000005</c:v>
+                  <c:v>0.71250000000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.75</c:v>
+                  <c:v>0.82105263157894737</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3339,64 +3339,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>3.1171875000000002E-2</c:v>
+                  <c:v>3.2484375000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.8906250000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10040625</c:v>
+                  <c:v>9.6468749999999992E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12862500000000002</c:v>
+                  <c:v>0.1273125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16570312500000001</c:v>
+                  <c:v>0.15914062500000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.19884374999999999</c:v>
+                  <c:v>0.19293749999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.22279687499999998</c:v>
+                  <c:v>0.2205</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25462499999999999</c:v>
+                  <c:v>0.27562500000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.29826562499999998</c:v>
+                  <c:v>0.28054687499999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.315</c:v>
+                  <c:v>0.33140625000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.34649999999999997</c:v>
+                  <c:v>0.37898437499999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.38587499999999997</c:v>
+                  <c:v>0.39768749999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.41376562500000003</c:v>
+                  <c:v>0.44362499999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.46396874999999999</c:v>
+                  <c:v>0.45937499999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.477421875</c:v>
+                  <c:v>0.48726562499999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.54600000000000004</c:v>
+                  <c:v>0.49875000000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.58570312499999988</c:v>
+                  <c:v>0.56339062499999992</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.61424999999999996</c:v>
+                  <c:v>0.60834374999999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.65460937499999994</c:v>
+                  <c:v>0.64837499999999992</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.63656250000000003</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3515,64 +3515,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2.192307692307692E-2</c:v>
+                  <c:v>2.3769230769230768E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.8461538461538459E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7153846153846147E-2</c:v>
+                  <c:v>6.576923076923076E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.138461538461537E-2</c:v>
+                  <c:v>8.9538461538461525E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11653846153846152</c:v>
+                  <c:v>0.11999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.13153846153846152</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15992307692307692</c:v>
+                  <c:v>0.16799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17907692307692305</c:v>
+                  <c:v>0.18646153846153846</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21184615384615382</c:v>
+                  <c:v>0.20146153846153844</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23307692307692304</c:v>
+                  <c:v>0.23076923076923073</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25384615384615378</c:v>
+                  <c:v>0.24369230769230762</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.28799999999999998</c:v>
+                  <c:v>0.26584615384615379</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.28499999999999998</c:v>
+                  <c:v>0.30599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.31015384615384611</c:v>
+                  <c:v>0.3295384615384615</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.33923076923076917</c:v>
+                  <c:v>0.33230769230769225</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.3692307692307692</c:v>
+                  <c:v>0.36553846153846148</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.38053846153846155</c:v>
+                  <c:v>0.37269230769230771</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.43615384615384611</c:v>
+                  <c:v>0.41953846153846153</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.42969230769230765</c:v>
+                  <c:v>0.44284615384615378</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.44769230769230761</c:v>
+                  <c:v>0.45692307692307682</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3689,64 +3689,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.35E-2</c:v>
+                  <c:v>1.3363636363636362E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8363636363636362E-2</c:v>
+                  <c:v>2.809090909090909E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2954545454545447E-2</c:v>
+                  <c:v>4.1727272727272717E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.618181818181818E-2</c:v>
+                  <c:v>5.7272727272727267E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.7499999999999991E-2</c:v>
+                  <c:v>6.6818181818181818E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9363636363636345E-2</c:v>
+                  <c:v>8.5090909090909078E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1636363636363627E-2</c:v>
+                  <c:v>9.0681818181818169E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10363636363636364</c:v>
+                  <c:v>0.10581818181818181</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12886363636363637</c:v>
+                  <c:v>0.11904545454545454</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.13499999999999998</c:v>
+                  <c:v>0.13909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14699999999999999</c:v>
+                  <c:v>0.153</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16036363636363635</c:v>
+                  <c:v>0.16854545454545453</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.17727272727272728</c:v>
+                  <c:v>0.17372727272727273</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.18136363636363634</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.19431818181818181</c:v>
+                  <c:v>0.20863636363636362</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.20945454545454545</c:v>
+                  <c:v>0.2138181818181818</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.24109090909090905</c:v>
+                  <c:v>0.22486363636363632</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.23318181818181818</c:v>
+                  <c:v>0.25772727272727275</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.24872727272727274</c:v>
+                  <c:v>0.25650000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.27272727272727271</c:v>
+                  <c:v>0.25909090909090909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3865,64 +3865,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.4045454545454545E-2</c:v>
+                  <c:v>1.3636363636363636E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8636363636363633E-2</c:v>
+                  <c:v>2.6727272727272725E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0909090909090902E-2</c:v>
+                  <c:v>4.2136363636363632E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2363636363636362E-2</c:v>
+                  <c:v>5.4545454545454543E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0227272727272722E-2</c:v>
+                  <c:v>6.8181818181818177E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.1818181818181804E-2</c:v>
+                  <c:v>7.9363636363636345E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.2590909090909085E-2</c:v>
+                  <c:v>9.8318181818181805E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10363636363636364</c:v>
+                  <c:v>0.11236363636363636</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.11659090909090909</c:v>
+                  <c:v>0.11781818181818182</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.14045454545454544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1515</c:v>
+                  <c:v>0.14249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16527272727272724</c:v>
+                  <c:v>0.16363636363636361</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.17904545454545454</c:v>
+                  <c:v>0.18436363636363637</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.20045454545454544</c:v>
+                  <c:v>0.18136363636363634</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.21477272727272725</c:v>
+                  <c:v>0.19431818181818181</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.22690909090909089</c:v>
+                  <c:v>0.22909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.22718181818181815</c:v>
+                  <c:v>0.24109090909090905</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.23318181818181818</c:v>
+                  <c:v>0.25281818181818183</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.25909090909090909</c:v>
+                  <c:v>0.26945454545454545</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.27272727272727271</c:v>
+                  <c:v>0.26181818181818178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4041,61 +4041,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>4.1447368421052627E-3</c:v>
+                  <c:v>3.7499999999999994E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.7368421052631565E-3</c:v>
+                  <c:v>8.2105263157894719E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.1605263157894737E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5315789473684208E-2</c:v>
+                  <c:v>1.6105263157894734E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8947368421052629E-2</c:v>
+                  <c:v>1.9144736842105263E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.368421052631579E-2</c:v>
+                  <c:v>2.2973684210526316E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8460526315789474E-2</c:v>
+                  <c:v>2.7907894736842104E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.189473684210526E-2</c:v>
+                  <c:v>3.2210526315789467E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5526315789473677E-2</c:v>
+                  <c:v>3.588157894736841E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0263157894736841E-2</c:v>
+                  <c:v>3.8289473684210526E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2118421052631576E-2</c:v>
+                  <c:v>4.3421052631578944E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.5473684210526319E-2</c:v>
+                  <c:v>4.9736842105263163E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.131578947368421E-2</c:v>
+                  <c:v>4.9776315789473682E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.3605263157894732E-2</c:v>
+                  <c:v>5.8026315789473683E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.8618421052631577E-2</c:v>
+                  <c:v>6.0986842105263152E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.5684210526315776E-2</c:v>
+                  <c:v>6.3157894736842093E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5763157894736843E-2</c:v>
+                  <c:v>6.7105263157894737E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.7499999999999991E-2</c:v>
+                  <c:v>7.0342105263157886E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.3499999999999996E-2</c:v>
+                  <c:v>7.4249999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>7.6578947368421052E-2</c:v>
@@ -5816,8 +5816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD913AE-747E-C341-AF89-CB2D285A6A4D}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A31"/>
+    <sheetView tabSelected="1" topLeftCell="P8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8077,59 +8077,59 @@
     <row r="57" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C57">
         <f ca="1">C21*RANDBETWEEN($C$52,$C$53)*0.01+C21</f>
-        <v>7.3923444976076558E-2</v>
+        <v>7.320574162679426E-2</v>
       </c>
       <c r="D57">
         <f t="shared" ref="D57:V67" ca="1" si="26">D21*RANDBETWEEN($C$52,$C$53)*0.01+D21</f>
-        <v>0.14928229665071771</v>
+        <v>0.14784688995215312</v>
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.22392344497607655</v>
+        <v>0.22177033492822965</v>
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.2755980861244019</v>
+        <v>0.29282296650717704</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.35885167464114831</v>
+        <v>0.36602870813397126</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.44354066985645929</v>
+        <v>0.40909090909090906</v>
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.51244019138755981</v>
+        <v>0.52751196172248804</v>
       </c>
       <c r="J57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.56267942583732056</v>
+        <v>0.58564593301435408</v>
       </c>
       <c r="K57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.63947368421052631</v>
+        <v>0.61363636363636365</v>
       </c>
       <c r="L57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.68181818181818177</v>
+        <v>0.75358851674641147</v>
       </c>
       <c r="M57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.82894736842105265</v>
+        <v>0.78157894736842104</v>
       </c>
       <c r="N57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.87846889952153107</v>
+        <v>0.84401913875598078</v>
       </c>
       <c r="O57">
         <f t="shared" ca="1" si="26"/>
-        <v>0.91435406698564592</v>
+        <v>0.88636363636363635</v>
       </c>
       <c r="P57">
         <f t="shared" ca="1" si="26"/>
-        <v>1.0349282296650717</v>
+        <v>1.0449760765550238</v>
       </c>
       <c r="Q57">
         <f t="shared" ca="1" si="26"/>
@@ -8137,57 +8137,57 @@
       </c>
       <c r="R57">
         <f t="shared" ca="1" si="26"/>
-        <v>1.1712918660287082</v>
+        <v>1.1253588516746411</v>
       </c>
       <c r="S57">
         <f t="shared" ca="1" si="26"/>
-        <v>1.1712918660287079</v>
+        <v>1.1956937799043061</v>
       </c>
       <c r="T57">
         <f t="shared" ca="1" si="26"/>
-        <v>1.2789473684210526</v>
+        <v>1.3306220095693782</v>
       </c>
       <c r="U57">
         <f t="shared" ca="1" si="26"/>
-        <v>1.4318181818181817</v>
+        <v>1.418181818181818</v>
       </c>
       <c r="V57">
         <f t="shared" ca="1" si="26"/>
-        <v>1.4784688995215309</v>
+        <v>1.5071770334928229</v>
       </c>
       <c r="X57">
         <f ca="1">SLOPE(C57:V57,$C$6:$V$6)/$B$3</f>
-        <v>19.345396985286179</v>
+        <v>19.45432960391409</v>
       </c>
     </row>
     <row r="58" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C58">
         <f t="shared" ref="C58:R67" ca="1" si="27">C22*RANDBETWEEN($C$52,$C$53)*0.01+C22</f>
-        <v>6.8807339449541288E-2</v>
+        <v>7.087155963302752E-2</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.13486238532110092</v>
+        <v>0.13211009174311927</v>
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.21467889908256879</v>
+        <v>0.19610091743119265</v>
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.26697247706422023</v>
+        <v>0.26422018348623855</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.34059633027522934</v>
+        <v>0.34747706422018348</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.4211009174311926</v>
+        <v>0.41284403669724767</v>
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.49128440366972481</v>
+        <v>0.48165137614678905</v>
       </c>
       <c r="J58">
         <f t="shared" ca="1" si="27"/>
@@ -8195,69 +8195,69 @@
       </c>
       <c r="K58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.61926605504587151</v>
+        <v>0.6316513761467889</v>
       </c>
       <c r="L58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.65366972477064222</v>
+        <v>0.72247706422018343</v>
       </c>
       <c r="M58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.726605504587156</v>
+        <v>0.74931192660550461</v>
       </c>
       <c r="N58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.82568807339449535</v>
+        <v>0.83394495412844027</v>
       </c>
       <c r="O58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.87660550458715591</v>
+        <v>0.88555045871559634</v>
       </c>
       <c r="P58">
         <f t="shared" ca="1" si="27"/>
-        <v>0.95366972477064227</v>
+        <v>0.92477064220183491</v>
       </c>
       <c r="Q58">
         <f t="shared" ca="1" si="27"/>
-        <v>1.0114678899082568</v>
+        <v>1.0837155963302751</v>
       </c>
       <c r="R58">
         <f t="shared" ca="1" si="27"/>
-        <v>1.0568807339449542</v>
+        <v>1.0788990825688074</v>
       </c>
       <c r="S58">
         <f t="shared" ca="1" si="26"/>
-        <v>1.1580275229357797</v>
+        <v>1.2048165137614679</v>
       </c>
       <c r="T58">
         <f t="shared" ca="1" si="26"/>
-        <v>1.1889908256880732</v>
+        <v>1.2633027522935778</v>
       </c>
       <c r="U58">
         <f t="shared" ca="1" si="26"/>
-        <v>1.3727064220183487</v>
+        <v>1.3596330275229358</v>
       </c>
       <c r="V58">
         <f t="shared" ca="1" si="26"/>
-        <v>1.3623853211009174</v>
+        <v>1.3211009174311927</v>
       </c>
       <c r="X58">
         <f t="shared" ref="X58:X67" ca="1" si="28">SLOPE(C58:V58,$C$6:$V$6)/$B$3</f>
-        <v>18.165275574256743</v>
+        <v>18.522314961716216</v>
       </c>
     </row>
     <row r="59" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C59">
         <f t="shared" ca="1" si="27"/>
-        <v>6.5791139240506322E-2</v>
+        <v>6.7784810126582273E-2</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.13424050632911391</v>
+        <v>0.13158227848101264</v>
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.20534810126582276</v>
+        <v>0.20734177215189872</v>
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="26"/>
@@ -8265,23 +8265,23 @@
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.34556962025316451</v>
+        <v>0.33892405063291131</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.37879746835443034</v>
+        <v>0.41468354430379745</v>
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.48379746835443038</v>
+        <v>0.45123417721518988</v>
       </c>
       <c r="J59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.54227848101265819</v>
+        <v>0.5156962025316455</v>
       </c>
       <c r="K59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.61604430379746833</v>
+        <v>0.59212025316455696</v>
       </c>
       <c r="L59">
         <f t="shared" ca="1" si="26"/>
@@ -8289,47 +8289,47 @@
       </c>
       <c r="M59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.72370253164556952</v>
+        <v>0.7602531645569619</v>
       </c>
       <c r="N59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.78151898734177205</v>
+        <v>0.78949367088607592</v>
       </c>
       <c r="O59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.82072784810126576</v>
+        <v>0.88120253164556961</v>
       </c>
       <c r="P59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.95829113924050624</v>
+        <v>0.92107594936708859</v>
       </c>
       <c r="Q59">
         <f t="shared" ca="1" si="26"/>
-        <v>0.99683544303797456</v>
+        <v>1.0367088607594936</v>
       </c>
       <c r="R59">
         <f t="shared" ca="1" si="26"/>
-        <v>1.0739240506329113</v>
+        <v>1.0101265822784808</v>
       </c>
       <c r="S59">
         <f t="shared" ca="1" si="26"/>
-        <v>1.1862341772151896</v>
+        <v>1.1749367088607592</v>
       </c>
       <c r="T59">
         <f t="shared" ca="1" si="26"/>
-        <v>1.2081645569620252</v>
+        <v>1.136392405063291</v>
       </c>
       <c r="U59">
         <f t="shared" ca="1" si="26"/>
-        <v>1.2374050632911391</v>
+        <v>1.3131645569620252</v>
       </c>
       <c r="V59">
         <f t="shared" ca="1" si="26"/>
-        <v>1.3025316455696201</v>
+        <v>1.2759493670886073</v>
       </c>
       <c r="X59">
         <f t="shared" ca="1" si="28"/>
-        <v>17.666355762824779</v>
+        <v>17.56189207195203</v>
       </c>
     </row>
     <row r="60" spans="3:24" x14ac:dyDescent="0.2">
@@ -8339,55 +8339,55 @@
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.1273469387755102</v>
+        <v>0.12612244897959182</v>
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.18183673469387757</v>
+        <v>0.19285714285714287</v>
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.24</v>
+        <v>0.2473469387755102</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.29081632653061223</v>
+        <v>0.3</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.36734693877551022</v>
+        <v>0.3563265306122449</v>
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.43285714285714288</v>
+        <v>0.43714285714285717</v>
       </c>
       <c r="J60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.48489795918367345</v>
+        <v>0.4946938775510204</v>
       </c>
       <c r="K60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.54</v>
+        <v>0.5234693877551021</v>
       </c>
       <c r="L60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.61224489795918369</v>
+        <v>0.61836734693877549</v>
       </c>
       <c r="M60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.69367346938775509</v>
+        <v>0.63979591836734695</v>
       </c>
       <c r="N60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.69795918367346943</v>
+        <v>0.7567346938775511</v>
       </c>
       <c r="O60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.80387755102040814</v>
+        <v>0.79591836734693877</v>
       </c>
       <c r="P60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.81428571428571439</v>
+        <v>0.84857142857142864</v>
       </c>
       <c r="Q60">
         <f t="shared" ca="1" si="26"/>
@@ -8395,113 +8395,113 @@
       </c>
       <c r="R60">
         <f t="shared" ca="1" si="26"/>
-        <v>0.9893877551020408</v>
+        <v>0.94040816326530607</v>
       </c>
       <c r="S60">
         <f t="shared" ca="1" si="26"/>
-        <v>1.0304081632653059</v>
+        <v>1.0199999999999998</v>
       </c>
       <c r="T60">
         <f t="shared" ca="1" si="26"/>
-        <v>1.08</v>
+        <v>1.0469387755102042</v>
       </c>
       <c r="U60">
         <f t="shared" ca="1" si="26"/>
-        <v>1.2214285714285713</v>
+        <v>1.1516326530612244</v>
       </c>
       <c r="V60">
         <f t="shared" ca="1" si="26"/>
-        <v>1.2122448979591838</v>
+        <v>1.1632653061224489</v>
       </c>
       <c r="X60">
         <f t="shared" ca="1" si="28"/>
-        <v>16.338928955040657</v>
+        <v>15.688936627282494</v>
       </c>
     </row>
     <row r="61" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C61">
         <f t="shared" ca="1" si="27"/>
-        <v>4.9655172413793101E-2</v>
+        <v>5.3275862068965514E-2</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.10758620689655173</v>
+        <v>0.10655172413793103</v>
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.15051724137931036</v>
+        <v>0.15362068965517242</v>
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.19655172413793104</v>
+        <v>0.20689655172413793</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.25862068965517243</v>
+        <v>0.26120689655172413</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.30103448275862071</v>
+        <v>0.29482758620689659</v>
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.34396551724137936</v>
+        <v>0.35120689655172421</v>
       </c>
       <c r="J61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.41379310344827586</v>
+        <v>0.43448275862068964</v>
       </c>
       <c r="K61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.47017241379310343</v>
+        <v>0.44689655172413789</v>
       </c>
       <c r="L61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.52758620689655178</v>
+        <v>0.50689655172413794</v>
       </c>
       <c r="M61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.58603448275862069</v>
+        <v>0.59172413793103451</v>
       </c>
       <c r="N61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.64551724137931032</v>
+        <v>0.60827586206896556</v>
       </c>
       <c r="O61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.66568965517241385</v>
+        <v>0.6925862068965517</v>
       </c>
       <c r="P61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.69517241379310357</v>
+        <v>0.72413793103448287</v>
       </c>
       <c r="Q61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.75258620689655176</v>
+        <v>0.7448275862068966</v>
       </c>
       <c r="R61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.79448275862068962</v>
+        <v>0.86896551724137927</v>
       </c>
       <c r="S61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.90568965517241384</v>
+        <v>0.83534482758620698</v>
       </c>
       <c r="T61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.96827586206896554</v>
+        <v>0.91241379310344828</v>
       </c>
       <c r="U61">
         <f t="shared" ca="1" si="26"/>
-        <v>0.98275862068965525</v>
+        <v>1.0024137931034482</v>
       </c>
       <c r="V61">
         <f t="shared" ca="1" si="26"/>
-        <v>1.0758620689655174</v>
+        <v>1.0241379310344829</v>
       </c>
       <c r="X61">
         <f t="shared" ca="1" si="28"/>
-        <v>14.059528130671508</v>
+        <v>13.720922997148044</v>
       </c>
     </row>
     <row r="62" spans="3:24" x14ac:dyDescent="0.2">
@@ -8511,89 +8511,89 @@
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="26"/>
-        <v>7.8947368421052641E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.12197368421052632</v>
+        <v>0.12315789473684212</v>
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.16105263157894739</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.20131578947368423</v>
+        <v>0.19736842105263158</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.23684210526315791</v>
+        <v>0.24631578947368424</v>
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.27907894736842109</v>
+        <v>0.28460526315789475</v>
       </c>
       <c r="J62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.30000000000000004</v>
+        <v>0.30947368421052635</v>
       </c>
       <c r="K62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.35526315789473684</v>
+        <v>0.34460526315789475</v>
       </c>
       <c r="L62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.38289473684210529</v>
+        <v>0.39473684210526316</v>
       </c>
       <c r="M62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.44289473684210529</v>
+        <v>0.43855263157894736</v>
       </c>
       <c r="N62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.45947368421052637</v>
+        <v>0.45473684210526316</v>
       </c>
       <c r="O62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.52342105263157901</v>
+        <v>0.50802631578947377</v>
       </c>
       <c r="P62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.54157894736842116</v>
+        <v>0.56368421052631579</v>
       </c>
       <c r="Q62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.62171052631578938</v>
+        <v>0.5625</v>
       </c>
       <c r="R62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.63789473684210529</v>
+        <v>0.63157894736842113</v>
       </c>
       <c r="S62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.65763157894736846</v>
+        <v>0.69789473684210535</v>
       </c>
       <c r="T62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.70342105263157895</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="U62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.74250000000000005</v>
+        <v>0.71250000000000002</v>
       </c>
       <c r="V62">
         <f t="shared" ca="1" si="26"/>
-        <v>0.75</v>
+        <v>0.82105263157894737</v>
       </c>
       <c r="X62">
         <f t="shared" ca="1" si="28"/>
-        <v>10.333043134151172</v>
+        <v>10.429125445191929</v>
       </c>
     </row>
     <row r="63" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C63">
         <f t="shared" ca="1" si="27"/>
-        <v>3.1171875000000002E-2</v>
+        <v>3.2484375000000003E-2</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="26"/>
@@ -8601,85 +8601,85 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.10040625</v>
+        <v>9.6468749999999992E-2</v>
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.12862500000000002</v>
+        <v>0.1273125</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.16570312500000001</v>
+        <v>0.15914062500000001</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.19884374999999999</v>
+        <v>0.19293749999999998</v>
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.22279687499999998</v>
+        <v>0.2205</v>
       </c>
       <c r="J63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.25462499999999999</v>
+        <v>0.27562500000000001</v>
       </c>
       <c r="K63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.29826562499999998</v>
+        <v>0.28054687499999997</v>
       </c>
       <c r="L63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.315</v>
+        <v>0.33140625000000001</v>
       </c>
       <c r="M63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.34649999999999997</v>
+        <v>0.37898437499999998</v>
       </c>
       <c r="N63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.38587499999999997</v>
+        <v>0.39768749999999997</v>
       </c>
       <c r="O63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.41376562500000003</v>
+        <v>0.44362499999999999</v>
       </c>
       <c r="P63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.46396874999999999</v>
+        <v>0.45937499999999998</v>
       </c>
       <c r="Q63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.477421875</v>
+        <v>0.48726562499999998</v>
       </c>
       <c r="R63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.54600000000000004</v>
+        <v>0.49875000000000003</v>
       </c>
       <c r="S63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.58570312499999988</v>
+        <v>0.56339062499999992</v>
       </c>
       <c r="T63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.61424999999999996</v>
+        <v>0.60834374999999996</v>
       </c>
       <c r="U63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.65460937499999994</v>
+        <v>0.64837499999999992</v>
       </c>
       <c r="V63">
         <f t="shared" ca="1" si="26"/>
-        <v>0.63656250000000003</v>
+        <v>0.63</v>
       </c>
       <c r="X63">
         <f t="shared" ca="1" si="28"/>
-        <v>8.9378947368421056</v>
+        <v>8.791315789473682</v>
       </c>
     </row>
     <row r="64" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C64">
         <f t="shared" ca="1" si="27"/>
-        <v>2.192307692307692E-2</v>
+        <v>2.3769230769230768E-2</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="26"/>
@@ -8687,15 +8687,15 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="26"/>
-        <v>6.7153846153846147E-2</v>
+        <v>6.576923076923076E-2</v>
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="26"/>
-        <v>9.138461538461537E-2</v>
+        <v>8.9538461538461525E-2</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.11653846153846152</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="26"/>
@@ -8703,117 +8703,117 @@
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.15992307692307692</v>
+        <v>0.16799999999999998</v>
       </c>
       <c r="J64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.17907692307692305</v>
+        <v>0.18646153846153846</v>
       </c>
       <c r="K64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.21184615384615382</v>
+        <v>0.20146153846153844</v>
       </c>
       <c r="L64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.23307692307692304</v>
+        <v>0.23076923076923073</v>
       </c>
       <c r="M64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.25384615384615378</v>
+        <v>0.24369230769230762</v>
       </c>
       <c r="N64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.28799999999999998</v>
+        <v>0.26584615384615379</v>
       </c>
       <c r="O64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.28499999999999998</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="P64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.31015384615384611</v>
+        <v>0.3295384615384615</v>
       </c>
       <c r="Q64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.33923076923076917</v>
+        <v>0.33230769230769225</v>
       </c>
       <c r="R64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.3692307692307692</v>
+        <v>0.36553846153846148</v>
       </c>
       <c r="S64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.38053846153846155</v>
+        <v>0.37269230769230771</v>
       </c>
       <c r="T64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.43615384615384611</v>
+        <v>0.41953846153846153</v>
       </c>
       <c r="U64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.42969230769230765</v>
+        <v>0.44284615384615378</v>
       </c>
       <c r="V64">
         <f t="shared" ca="1" si="26"/>
-        <v>0.44769230769230761</v>
+        <v>0.45692307692307682</v>
       </c>
       <c r="X64">
         <f t="shared" ca="1" si="28"/>
-        <v>6.0839791787160191</v>
+        <v>6.0880971659919032</v>
       </c>
     </row>
     <row r="65" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C65">
         <f t="shared" ca="1" si="27"/>
-        <v>1.35E-2</v>
+        <v>1.3363636363636362E-2</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="26"/>
-        <v>2.8363636363636362E-2</v>
+        <v>2.809090909090909E-2</v>
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="26"/>
-        <v>4.2954545454545447E-2</v>
+        <v>4.1727272727272717E-2</v>
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="26"/>
-        <v>5.618181818181818E-2</v>
+        <v>5.7272727272727267E-2</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="26"/>
-        <v>6.7499999999999991E-2</v>
+        <v>6.6818181818181818E-2</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="26"/>
-        <v>7.9363636363636345E-2</v>
+        <v>8.5090909090909078E-2</v>
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="26"/>
-        <v>9.1636363636363627E-2</v>
+        <v>9.0681818181818169E-2</v>
       </c>
       <c r="J65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.10363636363636364</v>
+        <v>0.10581818181818181</v>
       </c>
       <c r="K65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.12886363636363637</v>
+        <v>0.11904545454545454</v>
       </c>
       <c r="L65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.13499999999999998</v>
+        <v>0.13909090909090907</v>
       </c>
       <c r="M65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.14699999999999999</v>
+        <v>0.153</v>
       </c>
       <c r="N65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.16036363636363635</v>
+        <v>0.16854545454545453</v>
       </c>
       <c r="O65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.17727272727272728</v>
+        <v>0.17372727272727273</v>
       </c>
       <c r="P65">
         <f t="shared" ca="1" si="26"/>
@@ -8821,69 +8821,69 @@
       </c>
       <c r="Q65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.19431818181818181</v>
+        <v>0.20863636363636362</v>
       </c>
       <c r="R65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.20945454545454545</v>
+        <v>0.2138181818181818</v>
       </c>
       <c r="S65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.24109090909090905</v>
+        <v>0.22486363636363632</v>
       </c>
       <c r="T65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.23318181818181818</v>
+        <v>0.25772727272727275</v>
       </c>
       <c r="U65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.24872727272727274</v>
+        <v>0.25650000000000001</v>
       </c>
       <c r="V65">
         <f t="shared" ca="1" si="26"/>
-        <v>0.27272727272727271</v>
+        <v>0.25909090909090909</v>
       </c>
       <c r="X65">
         <f t="shared" ca="1" si="28"/>
-        <v>3.5343540669856464</v>
+        <v>3.5761585782638408</v>
       </c>
     </row>
     <row r="66" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C66">
         <f t="shared" ca="1" si="27"/>
-        <v>1.4045454545454545E-2</v>
+        <v>1.3636363636363636E-2</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="26"/>
-        <v>2.8636363636363633E-2</v>
+        <v>2.6727272727272725E-2</v>
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="26"/>
-        <v>4.0909090909090902E-2</v>
+        <v>4.2136363636363632E-2</v>
       </c>
       <c r="F66">
         <f t="shared" ca="1" si="26"/>
-        <v>5.2363636363636362E-2</v>
+        <v>5.4545454545454543E-2</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="26"/>
-        <v>7.0227272727272722E-2</v>
+        <v>6.8181818181818177E-2</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="26"/>
-        <v>8.1818181818181804E-2</v>
+        <v>7.9363636363636345E-2</v>
       </c>
       <c r="I66">
         <f t="shared" ca="1" si="26"/>
-        <v>9.2590909090909085E-2</v>
+        <v>9.8318181818181805E-2</v>
       </c>
       <c r="J66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.10363636363636364</v>
+        <v>0.11236363636363636</v>
       </c>
       <c r="K66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.11659090909090909</v>
+        <v>0.11781818181818182</v>
       </c>
       <c r="L66">
         <f t="shared" ca="1" si="26"/>
@@ -8891,57 +8891,57 @@
       </c>
       <c r="M66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.1515</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="N66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.16527272727272724</v>
+        <v>0.16363636363636361</v>
       </c>
       <c r="O66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.17904545454545454</v>
+        <v>0.18436363636363637</v>
       </c>
       <c r="P66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.20045454545454544</v>
+        <v>0.18136363636363634</v>
       </c>
       <c r="Q66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.21477272727272725</v>
+        <v>0.19431818181818181</v>
       </c>
       <c r="R66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.22690909090909089</v>
+        <v>0.22909090909090907</v>
       </c>
       <c r="S66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.22718181818181815</v>
+        <v>0.24109090909090905</v>
       </c>
       <c r="T66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.23318181818181818</v>
+        <v>0.25281818181818183</v>
       </c>
       <c r="U66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.25909090909090909</v>
+        <v>0.26945454545454545</v>
       </c>
       <c r="V66">
         <f t="shared" ca="1" si="26"/>
-        <v>0.27272727272727271</v>
+        <v>0.26181818181818178</v>
       </c>
       <c r="X66">
         <f t="shared" ca="1" si="28"/>
-        <v>3.6488585099111415</v>
+        <v>3.6716883116883117</v>
       </c>
     </row>
     <row r="67" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C67">
         <f t="shared" ca="1" si="27"/>
-        <v>4.1447368421052627E-3</v>
+        <v>3.7499999999999994E-3</v>
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="26"/>
-        <v>7.7368421052631565E-3</v>
+        <v>8.2105263157894719E-3</v>
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="26"/>
@@ -8949,67 +8949,67 @@
       </c>
       <c r="F67">
         <f t="shared" ca="1" si="26"/>
-        <v>1.5315789473684208E-2</v>
+        <v>1.6105263157894734E-2</v>
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="26"/>
-        <v>1.8947368421052629E-2</v>
+        <v>1.9144736842105263E-2</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="26"/>
-        <v>2.368421052631579E-2</v>
+        <v>2.2973684210526316E-2</v>
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="26"/>
-        <v>2.8460526315789474E-2</v>
+        <v>2.7907894736842104E-2</v>
       </c>
       <c r="J67">
         <f t="shared" ca="1" si="26"/>
-        <v>3.189473684210526E-2</v>
+        <v>3.2210526315789467E-2</v>
       </c>
       <c r="K67">
         <f t="shared" ca="1" si="26"/>
-        <v>3.5526315789473677E-2</v>
+        <v>3.588157894736841E-2</v>
       </c>
       <c r="L67">
         <f t="shared" ca="1" si="26"/>
-        <v>4.0263157894736841E-2</v>
+        <v>3.8289473684210526E-2</v>
       </c>
       <c r="M67">
         <f t="shared" ca="1" si="26"/>
-        <v>4.2118421052631576E-2</v>
+        <v>4.3421052631578944E-2</v>
       </c>
       <c r="N67">
         <f t="shared" ca="1" si="26"/>
-        <v>4.5473684210526319E-2</v>
+        <v>4.9736842105263163E-2</v>
       </c>
       <c r="O67">
         <f t="shared" ca="1" si="26"/>
-        <v>5.131578947368421E-2</v>
+        <v>4.9776315789473682E-2</v>
       </c>
       <c r="P67">
         <f t="shared" ca="1" si="26"/>
-        <v>5.3605263157894732E-2</v>
+        <v>5.8026315789473683E-2</v>
       </c>
       <c r="Q67">
         <f t="shared" ca="1" si="26"/>
-        <v>5.8618421052631577E-2</v>
+        <v>6.0986842105263152E-2</v>
       </c>
       <c r="R67">
         <f t="shared" ca="1" si="26"/>
-        <v>6.5684210526315776E-2</v>
+        <v>6.3157894736842093E-2</v>
       </c>
       <c r="S67">
         <f t="shared" ca="1" si="26"/>
-        <v>6.5763157894736843E-2</v>
+        <v>6.7105263157894737E-2</v>
       </c>
       <c r="T67">
         <f t="shared" ca="1" si="26"/>
-        <v>6.7499999999999991E-2</v>
+        <v>7.0342105263157886E-2</v>
       </c>
       <c r="U67">
         <f t="shared" ca="1" si="26"/>
-        <v>7.3499999999999996E-2</v>
+        <v>7.4249999999999997E-2</v>
       </c>
       <c r="V67">
         <f t="shared" ca="1" si="26"/>
@@ -9017,7 +9017,7 @@
       </c>
       <c r="X67">
         <f t="shared" ca="1" si="28"/>
-        <v>1.0269252077562325</v>
+        <v>1.0470360110803325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>